<commit_message>
Restructure to curl format
Main - NaverCrawler
Url info crawling - NaverCrawlerUrl
Curl info crawling - NaverCrawlerCurl

Updated the pkl using recent template
</commit_message>
<xml_diff>
--- a/data/Liberation_Price Tracker SKU list_v1 - Final.xlsx
+++ b/data/Liberation_Price Tracker SKU list_v1 - Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limdaekyoung/PycharmProjects/liberation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kang.y.5\OneDrive - Procter and Gamble\Documents\GitHub\liberation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35750474-E56F-8748-AE37-885A5432B81F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{35750474-E56F-8748-AE37-885A5432B81F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E206F708-9A8F-4001-92E1-F9D25D4F0660}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="740" windowWidth="29040" windowHeight="15840" tabRatio="779" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="779" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Tracking Product List_MSP" sheetId="7" r:id="rId1"/>
@@ -21,10 +21,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Price Tracking Product List_MSP'!$A$11:$BF$55</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1450,7 +1458,7 @@
     <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/6512752936/products?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=27600&amp;nvMid=6512752936&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=20&amp;pr=PC&amp;purchaseConditionSeq1=20040510&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SELLER_BY_PRICE&amp;catalogType=BRAND&amp;inflow=slbrc' \
+    <t>curl "https://search.shopping.naver.com/catalog/6512752936/products?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=27600&amp;nvMid=6512752936&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=20&amp;pr=PC&amp;purchaseConditionSeq1=20040510&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SELLER_BY_PRICE&amp;catalogType=BRAND&amp;inflow=slbrc" \
   -H 'Connection: keep-alive' \
   -H 'Accept: application/json, text/plain, */*' \
   -H 'User-Agent: Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
@@ -1462,7 +1470,6 @@
   -H 'Accept-Language: ko,en-US;q=0.9,en;q=0.8,ja;q=0.7,zh-CN;q=0.6,zh;q=0.5' \
   -H 'Cookie: ssm_au_c=kvugCAAD4BlH0l4vI72PkWec6JSvihl5qGMSV8o8zsxMgAAAA516KN/qJO/E5YgqAWbGFLM98x3S7y9J0WMJUhZ5mSrM=; ssm_au_c=kvugCAKOTAjCMAcPXx5SQAPPkKpk7QjI3AkyyjKlzN4ggAAAA1UexNKEFAuo6VvR/QX3GyWLpUhnbpMq1Sc/eAXmtMS0=; NNB=VCACQTT5ZKWF6; AD_SHP_BID=15; _sm_au_c=kvugCANzuCFMuUyiI0wDYAn3yFGx2+6JmQk+womGGdOUgAAAAVOtzVayeNX7lmhTpbHcEgt+v3whjYM0OveoCYn+nYRc=; JSESSIONID=4406F181691A0F541AFF7D86BB6126C3; NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; _naver_usersession_=5uprxhXwsGuZMdzmrxH38w==; nx_ssl=2; ASID=01ea394500000175bb1e0fbc00000065; page_uid=UIzRVlp0YiRsstTzN34ssssssBK-358452; spage_uid=UIzRVlp0YiRsstTzN34ssssssBK-358452; ncpa=95694|kheg7mq8|ede39d6220d82940e242c220ef3e185a56121c20|null|19d94815340e98611adc0cf9b15c103a9bbb2c1e' \
   --compressed</t>
-    <phoneticPr fontId="27" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1470,15 +1477,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1486,7 +1493,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1494,20 +1501,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1515,7 +1522,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1540,7 +1547,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1548,7 +1555,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1556,7 +1563,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1565,7 +1572,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1574,7 +1581,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1583,7 +1590,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1637,7 +1644,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1653,14 +1660,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1673,7 +1680,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1883,7 +1890,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1901,23 +1908,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -1998,7 +2005,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="1" applyFill="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="18" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2007,13 +2014,13 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
@@ -2030,6 +2037,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2079,11 +2089,16 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="28">
+    <cellStyle name="Accent1 2" xfId="3" xr:uid="{CD18BBF3-FE95-4D55-822D-0AA1A21D82CD}"/>
+    <cellStyle name="Comma [0] 2" xfId="21" xr:uid="{A70D06FA-B7BE-4404-AA98-EBB1B9CCEF8C}"/>
+    <cellStyle name="Comma 2" xfId="22" xr:uid="{9D90804A-5877-4326-AB4D-E82B030EF873}"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8"/>
+    <cellStyle name="Input 2" xfId="2" xr:uid="{F20D85D8-ABDA-4BA0-9A6B-522473105DCE}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E3027C87-3425-4354-A2E5-40D98544E226}"/>
+    <cellStyle name="Normal 2 2" xfId="19" xr:uid="{C0371AF8-5E3E-4743-AC06-6C5C6725E533}"/>
     <cellStyle name="강조색1 2" xfId="11" xr:uid="{A934E348-EA5B-4334-AF0A-1E05D501C3AF}"/>
     <cellStyle name="나쁨 2" xfId="9" xr:uid="{C2AC1E40-D9C4-4553-9EC2-4A44D1F99467}"/>
     <cellStyle name="백분율 2" xfId="23" xr:uid="{FB1E9176-C109-45C2-9F73-F2F505057D68}"/>
@@ -2094,7 +2109,6 @@
     <cellStyle name="쉼표 [0] 3" xfId="27" xr:uid="{8E904538-A644-418B-9A4A-87051DA35DB1}"/>
     <cellStyle name="쉼표 [0] 4" xfId="25" xr:uid="{29B49EEE-F2C3-4CCE-9864-F3C86953EF41}"/>
     <cellStyle name="입력 2" xfId="10" xr:uid="{09712B67-15E2-4842-82AA-E3DCB3572D0B}"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 12" xfId="17" xr:uid="{A379F59E-3062-4AB9-BA52-A3E4F139F891}"/>
     <cellStyle name="표준 2" xfId="8" xr:uid="{4AF07777-0331-4824-9328-4B8C4FA9D6B8}"/>
     <cellStyle name="표준 2 2" xfId="12" xr:uid="{2449B9C0-4AAE-4931-880D-596972103349}"/>
@@ -2105,13 +2119,6 @@
     <cellStyle name="표준 3" xfId="15" xr:uid="{A157B020-D4AF-4EAE-B97C-42B65F5881CF}"/>
     <cellStyle name="표준 4" xfId="4" xr:uid="{99D950CB-BAA1-4230-A942-4E456B745BA6}"/>
     <cellStyle name="표준 5" xfId="6" xr:uid="{0A89C352-BF6C-489E-9EAF-1AE4462E684E}"/>
-    <cellStyle name="하이퍼링크" xfId="18" builtinId="8"/>
-    <cellStyle name="Accent1 2" xfId="3" xr:uid="{CD18BBF3-FE95-4D55-822D-0AA1A21D82CD}"/>
-    <cellStyle name="Comma [0] 2" xfId="21" xr:uid="{A70D06FA-B7BE-4404-AA98-EBB1B9CCEF8C}"/>
-    <cellStyle name="Comma 2" xfId="22" xr:uid="{9D90804A-5877-4326-AB4D-E82B030EF873}"/>
-    <cellStyle name="Input 2" xfId="2" xr:uid="{F20D85D8-ABDA-4BA0-9A6B-522473105DCE}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{E3027C87-3425-4354-A2E5-40D98544E226}"/>
-    <cellStyle name="Normal 2 2" xfId="19" xr:uid="{C0371AF8-5E3E-4743-AC06-6C5C6725E533}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3522,7 +3529,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3822,66 +3829,66 @@
   <dimension ref="A1:BF55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="11" topLeftCell="L12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="11" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="17" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="17" customWidth="1"/>
     <col min="6" max="6" width="9" style="17" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="17" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="76.6640625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="18.5" style="17" customWidth="1"/>
-    <col min="16" max="16" width="18.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="76.7109375" style="17" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="67.5" style="17" customWidth="1"/>
-    <col min="20" max="20" width="70.33203125" style="17" customWidth="1"/>
-    <col min="21" max="21" width="20.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.33203125" style="17" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" style="17" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" style="17" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="67.42578125" style="17" customWidth="1"/>
+    <col min="20" max="20" width="70.28515625" style="17" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" style="17" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" style="17" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="17" customWidth="1"/>
     <col min="25" max="28" width="23" style="17" customWidth="1"/>
     <col min="29" max="29" width="14" style="17" customWidth="1"/>
     <col min="30" max="30" width="30" style="17" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="30" style="17" customWidth="1"/>
-    <col min="32" max="32" width="23.5" style="17" customWidth="1"/>
-    <col min="33" max="33" width="20.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.5" style="17" customWidth="1"/>
-    <col min="36" max="36" width="19.33203125" style="17" customWidth="1"/>
-    <col min="37" max="37" width="17.33203125" style="17" customWidth="1"/>
-    <col min="38" max="38" width="20.5" style="17" customWidth="1"/>
-    <col min="39" max="39" width="18.1640625" style="17" customWidth="1"/>
-    <col min="40" max="40" width="20.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.42578125" style="17" customWidth="1"/>
+    <col min="33" max="33" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.42578125" style="17" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" style="17" customWidth="1"/>
+    <col min="37" max="37" width="17.28515625" style="17" customWidth="1"/>
+    <col min="38" max="38" width="20.42578125" style="17" customWidth="1"/>
+    <col min="39" max="39" width="18.140625" style="17" customWidth="1"/>
+    <col min="40" max="40" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="42" max="45" width="23" style="17" customWidth="1"/>
     <col min="46" max="46" width="14" style="17" customWidth="1"/>
     <col min="47" max="47" width="30" style="17" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="30" style="17" customWidth="1"/>
-    <col min="49" max="49" width="23.5" style="17" customWidth="1"/>
-    <col min="50" max="50" width="20.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.42578125" style="17" customWidth="1"/>
+    <col min="50" max="50" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="22" style="17" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="18.5" style="17" customWidth="1"/>
-    <col min="53" max="53" width="19.33203125" style="17" customWidth="1"/>
-    <col min="54" max="54" width="17.33203125" style="17" customWidth="1"/>
-    <col min="55" max="55" width="20.5" style="17" customWidth="1"/>
-    <col min="56" max="56" width="18.1640625" style="17" customWidth="1"/>
-    <col min="57" max="57" width="20.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.42578125" style="17" customWidth="1"/>
+    <col min="53" max="53" width="19.28515625" style="17" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" style="17" customWidth="1"/>
+    <col min="55" max="55" width="20.42578125" style="17" customWidth="1"/>
+    <col min="56" max="56" width="18.140625" style="17" customWidth="1"/>
+    <col min="57" max="57" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="59" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -3974,10 +3981,10 @@
       <c r="V8" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="W8" s="40" t="s">
+      <c r="W8" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="X8" s="40"/>
+      <c r="X8" s="41"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
@@ -4029,149 +4036,149 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:58" ht="16">
+    <row r="9" spans="1:58" ht="15.75">
       <c r="A9" s="7"/>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="44" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="44"/>
+      <c r="Y9" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
-      <c r="AB9" s="45"/>
-      <c r="AC9" s="45"/>
-      <c r="AD9" s="45"/>
-      <c r="AE9" s="45"/>
-      <c r="AF9" s="45"/>
-      <c r="AG9" s="45"/>
-      <c r="AH9" s="45"/>
-      <c r="AI9" s="45"/>
-      <c r="AJ9" s="45"/>
-      <c r="AK9" s="45"/>
-      <c r="AL9" s="45"/>
-      <c r="AM9" s="45"/>
-      <c r="AN9" s="45"/>
-      <c r="AO9" s="46"/>
-      <c r="AP9" s="47" t="s">
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="46"/>
+      <c r="AF9" s="46"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="46"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="46"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="46"/>
+      <c r="AM9" s="46"/>
+      <c r="AN9" s="46"/>
+      <c r="AO9" s="47"/>
+      <c r="AP9" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="AQ9" s="48"/>
-      <c r="AR9" s="48"/>
-      <c r="AS9" s="48"/>
-      <c r="AT9" s="48"/>
-      <c r="AU9" s="48"/>
-      <c r="AV9" s="48"/>
-      <c r="AW9" s="48"/>
-      <c r="AX9" s="48"/>
-      <c r="AY9" s="48"/>
-      <c r="AZ9" s="48"/>
-      <c r="BA9" s="48"/>
-      <c r="BB9" s="48"/>
-      <c r="BC9" s="48"/>
-      <c r="BD9" s="48"/>
-      <c r="BE9" s="48"/>
-      <c r="BF9" s="49"/>
+      <c r="AQ9" s="49"/>
+      <c r="AR9" s="49"/>
+      <c r="AS9" s="49"/>
+      <c r="AT9" s="49"/>
+      <c r="AU9" s="49"/>
+      <c r="AV9" s="49"/>
+      <c r="AW9" s="49"/>
+      <c r="AX9" s="49"/>
+      <c r="AY9" s="49"/>
+      <c r="AZ9" s="49"/>
+      <c r="BA9" s="49"/>
+      <c r="BB9" s="49"/>
+      <c r="BC9" s="49"/>
+      <c r="BD9" s="49"/>
+      <c r="BE9" s="49"/>
+      <c r="BF9" s="50"/>
     </row>
     <row r="10" spans="1:58">
       <c r="A10" s="4"/>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="51" t="s">
         <v>313</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="38" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="39" t="s">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="37" t="s">
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="37"/>
-      <c r="AD10" s="38" t="s">
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="39" t="s">
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
+      <c r="AG10" s="39"/>
+      <c r="AH10" s="39"/>
+      <c r="AI10" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="AJ10" s="39"/>
-      <c r="AK10" s="39"/>
-      <c r="AL10" s="39"/>
-      <c r="AM10" s="39"/>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="39"/>
-      <c r="AP10" s="37" t="s">
+      <c r="AJ10" s="40"/>
+      <c r="AK10" s="40"/>
+      <c r="AL10" s="40"/>
+      <c r="AM10" s="40"/>
+      <c r="AN10" s="40"/>
+      <c r="AO10" s="40"/>
+      <c r="AP10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="AQ10" s="37"/>
-      <c r="AR10" s="37"/>
-      <c r="AS10" s="37"/>
-      <c r="AT10" s="37"/>
-      <c r="AU10" s="38" t="s">
+      <c r="AQ10" s="38"/>
+      <c r="AR10" s="38"/>
+      <c r="AS10" s="38"/>
+      <c r="AT10" s="38"/>
+      <c r="AU10" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AV10" s="38"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="39" t="s">
+      <c r="AV10" s="39"/>
+      <c r="AW10" s="39"/>
+      <c r="AX10" s="39"/>
+      <c r="AY10" s="39"/>
+      <c r="AZ10" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="BA10" s="39"/>
-      <c r="BB10" s="39"/>
-      <c r="BC10" s="39"/>
-      <c r="BD10" s="39"/>
-      <c r="BE10" s="39"/>
-      <c r="BF10" s="39"/>
+      <c r="BA10" s="40"/>
+      <c r="BB10" s="40"/>
+      <c r="BC10" s="40"/>
+      <c r="BD10" s="40"/>
+      <c r="BE10" s="40"/>
+      <c r="BF10" s="40"/>
     </row>
     <row r="11" spans="1:58">
       <c r="A11" s="10" t="s">
@@ -4349,7 +4356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:58" s="16" customFormat="1" ht="409.6">
+    <row r="12" spans="1:58" s="16" customFormat="1" ht="409.5">
       <c r="A12" s="16">
         <v>1</v>
       </c>
@@ -4384,7 +4391,7 @@
       <c r="L12" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="M12" s="53" t="s">
+      <c r="M12" s="37" t="s">
         <v>455</v>
       </c>
       <c r="N12" s="16">
@@ -4491,7 +4498,7 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="14" spans="1:58" s="16" customFormat="1" ht="17">
+    <row r="14" spans="1:58" s="16" customFormat="1">
       <c r="A14" s="16">
         <v>3</v>
       </c>
@@ -4561,7 +4568,7 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="15" spans="1:58" s="16" customFormat="1" ht="17">
+    <row r="15" spans="1:58" s="16" customFormat="1">
       <c r="A15" s="16">
         <v>4</v>
       </c>
@@ -4631,7 +4638,7 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="16" customFormat="1" ht="17">
+    <row r="16" spans="1:58" s="16" customFormat="1">
       <c r="A16" s="16">
         <v>5</v>
       </c>
@@ -4701,7 +4708,7 @@
         <v>19400</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="17" spans="1:27" s="16" customFormat="1">
       <c r="A17" s="16">
         <v>6</v>
       </c>
@@ -4771,7 +4778,7 @@
         <v>19400</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="18" spans="1:27" s="16" customFormat="1">
       <c r="A18" s="16">
         <v>7</v>
       </c>
@@ -4841,7 +4848,7 @@
         <v>19400</v>
       </c>
     </row>
-    <row r="19" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="19" spans="1:27" s="16" customFormat="1">
       <c r="A19" s="16">
         <v>8</v>
       </c>
@@ -4911,7 +4918,7 @@
         <v>10300</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="20" spans="1:27" s="16" customFormat="1">
       <c r="A20" s="16">
         <v>9</v>
       </c>
@@ -4981,7 +4988,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="21" spans="1:27" s="16" customFormat="1">
       <c r="A21" s="16">
         <v>10</v>
       </c>
@@ -5053,7 +5060,7 @@
         <v>12900</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="22" spans="1:27" s="16" customFormat="1">
       <c r="A22" s="16">
         <v>11</v>
       </c>
@@ -5125,7 +5132,7 @@
         <v>12900</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="23" spans="1:27" s="16" customFormat="1">
       <c r="A23" s="16">
         <v>12</v>
       </c>
@@ -5197,7 +5204,7 @@
         <v>12900</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="24" spans="1:27" s="16" customFormat="1">
       <c r="A24" s="16">
         <v>13</v>
       </c>
@@ -5269,7 +5276,7 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="25" spans="1:27" s="16" customFormat="1">
       <c r="A25" s="16">
         <v>14</v>
       </c>
@@ -5341,7 +5348,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="26" spans="1:27" s="16" customFormat="1">
       <c r="A26" s="16">
         <v>15</v>
       </c>
@@ -5413,7 +5420,7 @@
         <v>17900</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="27" spans="1:27" s="16" customFormat="1">
       <c r="A27" s="16">
         <v>16</v>
       </c>
@@ -5486,7 +5493,7 @@
       </c>
       <c r="Y27" s="31"/>
     </row>
-    <row r="28" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="28" spans="1:27" s="16" customFormat="1">
       <c r="A28" s="16">
         <v>17</v>
       </c>
@@ -5558,7 +5565,7 @@
         <v>17900</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="29" spans="1:27" s="16" customFormat="1">
       <c r="A29" s="16">
         <v>18</v>
       </c>
@@ -5630,7 +5637,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="30" spans="1:27" s="16" customFormat="1">
       <c r="A30" s="16">
         <v>19</v>
       </c>
@@ -5702,7 +5709,7 @@
         <v>16900</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="31" spans="1:27" s="16" customFormat="1">
       <c r="A31" s="16">
         <v>20</v>
       </c>
@@ -5774,7 +5781,7 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="32" spans="1:27" s="16" customFormat="1">
       <c r="A32" s="16">
         <v>21</v>
       </c>
@@ -5811,7 +5818,7 @@
       </c>
       <c r="M32" s="27"/>
       <c r="N32" s="16">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O32" s="16">
         <v>1</v>
@@ -5848,7 +5855,7 @@
       <c r="Z32" s="31"/>
       <c r="AA32" s="31"/>
     </row>
-    <row r="33" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="33" spans="1:27" s="16" customFormat="1">
       <c r="A33" s="16">
         <v>22</v>
       </c>
@@ -5922,7 +5929,7 @@
       <c r="Z33" s="31"/>
       <c r="AA33" s="31"/>
     </row>
-    <row r="34" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="34" spans="1:27" s="16" customFormat="1">
       <c r="A34" s="16">
         <v>23</v>
       </c>
@@ -5996,7 +6003,7 @@
       <c r="Z34" s="31"/>
       <c r="AA34" s="31"/>
     </row>
-    <row r="35" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="35" spans="1:27" s="16" customFormat="1">
       <c r="A35" s="16">
         <v>24</v>
       </c>
@@ -6070,7 +6077,7 @@
       <c r="Z35" s="31"/>
       <c r="AA35" s="31"/>
     </row>
-    <row r="36" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="36" spans="1:27" s="16" customFormat="1">
       <c r="A36" s="16">
         <v>25</v>
       </c>
@@ -6144,7 +6151,7 @@
       <c r="Z36" s="31"/>
       <c r="AA36" s="31"/>
     </row>
-    <row r="37" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="37" spans="1:27" s="16" customFormat="1">
       <c r="A37" s="16">
         <v>26</v>
       </c>
@@ -6218,7 +6225,7 @@
       <c r="Z37" s="31"/>
       <c r="AA37" s="31"/>
     </row>
-    <row r="38" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="38" spans="1:27" s="16" customFormat="1">
       <c r="A38" s="16">
         <v>27</v>
       </c>
@@ -6292,7 +6299,7 @@
       <c r="Z38" s="31"/>
       <c r="AA38" s="31"/>
     </row>
-    <row r="39" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="39" spans="1:27" s="16" customFormat="1">
       <c r="A39" s="16">
         <v>28</v>
       </c>
@@ -6366,7 +6373,7 @@
       <c r="Z39" s="31"/>
       <c r="AA39" s="31"/>
     </row>
-    <row r="40" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="40" spans="1:27" s="16" customFormat="1">
       <c r="A40" s="16">
         <v>29</v>
       </c>
@@ -6440,7 +6447,7 @@
       <c r="Z40" s="31"/>
       <c r="AA40" s="31"/>
     </row>
-    <row r="41" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="41" spans="1:27" s="16" customFormat="1">
       <c r="A41" s="16">
         <v>30</v>
       </c>
@@ -6514,7 +6521,7 @@
       <c r="Z41" s="31"/>
       <c r="AA41" s="31"/>
     </row>
-    <row r="42" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="42" spans="1:27" s="16" customFormat="1">
       <c r="A42" s="16">
         <v>31</v>
       </c>
@@ -6588,7 +6595,7 @@
       <c r="Z42" s="31"/>
       <c r="AA42" s="31"/>
     </row>
-    <row r="43" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="43" spans="1:27" s="16" customFormat="1">
       <c r="A43" s="16">
         <v>32</v>
       </c>
@@ -6662,7 +6669,7 @@
       <c r="Z43" s="31"/>
       <c r="AA43" s="31"/>
     </row>
-    <row r="44" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="44" spans="1:27" s="16" customFormat="1">
       <c r="A44" s="16">
         <v>33</v>
       </c>
@@ -6736,7 +6743,7 @@
       <c r="Z44" s="31"/>
       <c r="AA44" s="31"/>
     </row>
-    <row r="45" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="45" spans="1:27" s="16" customFormat="1">
       <c r="A45" s="16">
         <v>34</v>
       </c>
@@ -6812,7 +6819,7 @@
       <c r="Z45" s="31"/>
       <c r="AA45" s="31"/>
     </row>
-    <row r="46" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="46" spans="1:27" s="16" customFormat="1">
       <c r="A46" s="16">
         <v>35</v>
       </c>
@@ -6889,7 +6896,7 @@
       <c r="Z46" s="31"/>
       <c r="AA46" s="31"/>
     </row>
-    <row r="47" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="47" spans="1:27" s="16" customFormat="1">
       <c r="A47" s="16">
         <v>36</v>
       </c>
@@ -6966,7 +6973,7 @@
       <c r="Z47" s="31"/>
       <c r="AA47" s="31"/>
     </row>
-    <row r="48" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="48" spans="1:27" s="16" customFormat="1">
       <c r="A48" s="16">
         <v>37</v>
       </c>
@@ -7043,7 +7050,7 @@
       <c r="Z48" s="31"/>
       <c r="AA48" s="31"/>
     </row>
-    <row r="49" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="49" spans="1:27" s="16" customFormat="1">
       <c r="A49" s="16">
         <v>38</v>
       </c>
@@ -7120,7 +7127,7 @@
       <c r="Z49" s="31"/>
       <c r="AA49" s="31"/>
     </row>
-    <row r="50" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="50" spans="1:27" s="16" customFormat="1">
       <c r="A50" s="16">
         <v>39</v>
       </c>
@@ -7197,7 +7204,7 @@
       <c r="Z50" s="31"/>
       <c r="AA50" s="31"/>
     </row>
-    <row r="51" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="51" spans="1:27" s="16" customFormat="1">
       <c r="A51" s="16">
         <v>40</v>
       </c>
@@ -7274,7 +7281,7 @@
       <c r="Z51" s="31"/>
       <c r="AA51" s="31"/>
     </row>
-    <row r="52" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="52" spans="1:27" s="16" customFormat="1">
       <c r="A52" s="16">
         <v>41</v>
       </c>
@@ -7350,7 +7357,7 @@
       <c r="Z52" s="31"/>
       <c r="AA52" s="31"/>
     </row>
-    <row r="53" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="53" spans="1:27" s="16" customFormat="1">
       <c r="A53" s="16">
         <v>42</v>
       </c>
@@ -7427,7 +7434,7 @@
       <c r="Z53" s="31"/>
       <c r="AA53" s="31"/>
     </row>
-    <row r="54" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="54" spans="1:27" s="16" customFormat="1">
       <c r="A54" s="16">
         <v>43</v>
       </c>
@@ -7504,7 +7511,7 @@
       <c r="Z54" s="31"/>
       <c r="AA54" s="31"/>
     </row>
-    <row r="55" spans="1:27" s="16" customFormat="1" ht="17">
+    <row r="55" spans="1:27" s="16" customFormat="1">
       <c r="A55" s="16">
         <v>44</v>
       </c>
@@ -7701,14 +7708,14 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="172.5" customWidth="1"/>
-    <col min="3" max="3" width="65.5" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="172.42578125" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>130</v>
       </c>
@@ -7741,9 +7748,9 @@
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="20">
+    <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>131</v>
       </c>
@@ -7768,16 +7775,16 @@
       <selection activeCell="C10" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29.5" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>